<commit_message>
Added rxd to TimeStream and InfluxDB
</commit_message>
<xml_diff>
--- a/RXD/logger mf4 data.xlsx
+++ b/RXD/logger mf4 data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Current Projects\SharpInfluxComponents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Current Projects\SharpInfluxComponents\RXD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C93C9C2A-4204-4A2D-BB43-805FC8CA8C9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDAAF983-CBA7-4E00-A692-F83C8E28862D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="750" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="750" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RXD" sheetId="2" r:id="rId1"/>
@@ -1038,6 +1038,57 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="26" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1047,9 +1098,6 @@
     <xf numFmtId="0" fontId="8" fillId="26" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1059,54 +1107,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1133,12 +1139,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1491,8 +1491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BB56"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="V30" sqref="V30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q26" sqref="Q26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1509,20 +1509,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:54" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="103" t="s">
+      <c r="B1" s="107" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="103"/>
-      <c r="AU1" s="103" t="s">
+      <c r="C1" s="107"/>
+      <c r="AU1" s="107" t="s">
         <v>100</v>
       </c>
-      <c r="AV1" s="103"/>
-      <c r="AW1" s="103"/>
-      <c r="AX1" s="103"/>
-      <c r="AY1" s="103"/>
-      <c r="AZ1" s="103"/>
-      <c r="BA1" s="103"/>
-      <c r="BB1" s="103"/>
+      <c r="AV1" s="107"/>
+      <c r="AW1" s="107"/>
+      <c r="AX1" s="107"/>
+      <c r="AY1" s="107"/>
+      <c r="AZ1" s="107"/>
+      <c r="BA1" s="107"/>
+      <c r="BB1" s="107"/>
     </row>
     <row r="2" spans="1:54" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="56"/>
@@ -1538,15 +1538,15 @@
       <c r="AU3" s="85" t="s">
         <v>89</v>
       </c>
-      <c r="AV3" s="104" t="s">
+      <c r="AV3" s="120" t="s">
         <v>99</v>
       </c>
-      <c r="AW3" s="105"/>
-      <c r="AX3" s="105"/>
-      <c r="AY3" s="105"/>
-      <c r="AZ3" s="105"/>
-      <c r="BA3" s="105"/>
-      <c r="BB3" s="106"/>
+      <c r="AW3" s="121"/>
+      <c r="AX3" s="121"/>
+      <c r="AY3" s="121"/>
+      <c r="AZ3" s="121"/>
+      <c r="BA3" s="121"/>
+      <c r="BB3" s="122"/>
     </row>
     <row r="4" spans="1:54" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
@@ -1558,15 +1558,15 @@
       <c r="AU4" s="85" t="s">
         <v>90</v>
       </c>
-      <c r="AV4" s="104" t="s">
+      <c r="AV4" s="120" t="s">
         <v>95</v>
       </c>
-      <c r="AW4" s="105"/>
-      <c r="AX4" s="105"/>
-      <c r="AY4" s="105"/>
-      <c r="AZ4" s="105"/>
-      <c r="BA4" s="105"/>
-      <c r="BB4" s="106"/>
+      <c r="AW4" s="121"/>
+      <c r="AX4" s="121"/>
+      <c r="AY4" s="121"/>
+      <c r="AZ4" s="121"/>
+      <c r="BA4" s="121"/>
+      <c r="BB4" s="122"/>
     </row>
     <row r="5" spans="1:54" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
@@ -1578,15 +1578,15 @@
       <c r="AU5" s="85" t="s">
         <v>91</v>
       </c>
-      <c r="AV5" s="104" t="s">
+      <c r="AV5" s="120" t="s">
         <v>96</v>
       </c>
-      <c r="AW5" s="105"/>
-      <c r="AX5" s="105"/>
-      <c r="AY5" s="105"/>
-      <c r="AZ5" s="105"/>
-      <c r="BA5" s="105"/>
-      <c r="BB5" s="106"/>
+      <c r="AW5" s="121"/>
+      <c r="AX5" s="121"/>
+      <c r="AY5" s="121"/>
+      <c r="AZ5" s="121"/>
+      <c r="BA5" s="121"/>
+      <c r="BB5" s="122"/>
     </row>
     <row r="6" spans="1:54" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
@@ -1598,84 +1598,84 @@
       <c r="AU6" s="85" t="s">
         <v>92</v>
       </c>
-      <c r="AV6" s="104" t="s">
+      <c r="AV6" s="120" t="s">
         <v>97</v>
       </c>
-      <c r="AW6" s="105"/>
-      <c r="AX6" s="105"/>
-      <c r="AY6" s="105"/>
-      <c r="AZ6" s="105"/>
-      <c r="BA6" s="105"/>
-      <c r="BB6" s="106"/>
+      <c r="AW6" s="121"/>
+      <c r="AX6" s="121"/>
+      <c r="AY6" s="121"/>
+      <c r="AZ6" s="121"/>
+      <c r="BA6" s="121"/>
+      <c r="BB6" s="122"/>
     </row>
     <row r="7" spans="1:54" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H7" s="7"/>
       <c r="AU7" s="85" t="s">
         <v>88</v>
       </c>
-      <c r="AV7" s="132" t="s">
+      <c r="AV7" s="123" t="s">
         <v>98</v>
       </c>
-      <c r="AW7" s="132"/>
-      <c r="AX7" s="132"/>
-      <c r="AY7" s="132"/>
-      <c r="AZ7" s="132"/>
-      <c r="BA7" s="132"/>
-      <c r="BB7" s="132"/>
+      <c r="AW7" s="123"/>
+      <c r="AX7" s="123"/>
+      <c r="AY7" s="123"/>
+      <c r="AZ7" s="123"/>
+      <c r="BA7" s="123"/>
+      <c r="BB7" s="123"/>
     </row>
     <row r="8" spans="1:54" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H8" s="7"/>
       <c r="AU8" s="85" t="s">
         <v>110</v>
       </c>
-      <c r="AV8" s="132" t="s">
+      <c r="AV8" s="123" t="s">
         <v>112</v>
       </c>
-      <c r="AW8" s="132"/>
-      <c r="AX8" s="132"/>
-      <c r="AY8" s="132"/>
-      <c r="AZ8" s="132"/>
-      <c r="BA8" s="132"/>
-      <c r="BB8" s="132"/>
+      <c r="AW8" s="123"/>
+      <c r="AX8" s="123"/>
+      <c r="AY8" s="123"/>
+      <c r="AZ8" s="123"/>
+      <c r="BA8" s="123"/>
+      <c r="BB8" s="123"/>
     </row>
     <row r="9" spans="1:54" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H9" s="7"/>
       <c r="AU9" s="85" t="s">
         <v>111</v>
       </c>
-      <c r="AV9" s="132" t="s">
+      <c r="AV9" s="123" t="s">
         <v>113</v>
       </c>
-      <c r="AW9" s="132"/>
-      <c r="AX9" s="132"/>
-      <c r="AY9" s="132"/>
-      <c r="AZ9" s="132"/>
-      <c r="BA9" s="132"/>
-      <c r="BB9" s="132"/>
+      <c r="AW9" s="123"/>
+      <c r="AX9" s="123"/>
+      <c r="AY9" s="123"/>
+      <c r="AZ9" s="123"/>
+      <c r="BA9" s="123"/>
+      <c r="BB9" s="123"/>
     </row>
     <row r="10" spans="1:54" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H10" s="7"/>
       <c r="AU10" s="85" t="s">
         <v>114</v>
       </c>
-      <c r="AV10" s="132" t="s">
+      <c r="AV10" s="123" t="s">
         <v>115</v>
       </c>
-      <c r="AW10" s="132"/>
-      <c r="AX10" s="132"/>
-      <c r="AY10" s="132"/>
-      <c r="AZ10" s="132"/>
-      <c r="BA10" s="132"/>
-      <c r="BB10" s="132"/>
+      <c r="AW10" s="123"/>
+      <c r="AX10" s="123"/>
+      <c r="AY10" s="123"/>
+      <c r="AZ10" s="123"/>
+      <c r="BA10" s="123"/>
+      <c r="BB10" s="123"/>
     </row>
     <row r="11" spans="1:54" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H11" s="7"/>
     </row>
     <row r="12" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="D12" s="118" t="s">
+      <c r="D12" s="112" t="s">
         <v>41</v>
       </c>
-      <c r="E12" s="118"/>
+      <c r="E12" s="112"/>
       <c r="F12" s="53"/>
       <c r="G12" s="29"/>
       <c r="H12" s="53"/>
@@ -1717,10 +1717,10 @@
       <c r="AR12" s="53"/>
     </row>
     <row r="13" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="D13" s="119" t="s">
+      <c r="D13" s="113" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="119"/>
+      <c r="E13" s="113"/>
       <c r="F13" s="54"/>
       <c r="G13" s="29"/>
       <c r="H13" s="31"/>
@@ -1806,7 +1806,7 @@
     </row>
     <row r="15" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A15" s="23"/>
-      <c r="B15" s="117" t="s">
+      <c r="B15" s="102" t="s">
         <v>4</v>
       </c>
       <c r="C15" s="43"/>
@@ -1856,12 +1856,12 @@
     </row>
     <row r="16" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A16" s="23"/>
-      <c r="B16" s="117"/>
+      <c r="B16" s="102"/>
       <c r="C16" s="23"/>
-      <c r="D16" s="120" t="s">
+      <c r="D16" s="114" t="s">
         <v>31</v>
       </c>
-      <c r="E16" s="120"/>
+      <c r="E16" s="114"/>
       <c r="F16" s="32"/>
       <c r="G16" s="27"/>
       <c r="H16" s="23"/>
@@ -1871,7 +1871,7 @@
     </row>
     <row r="17" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A17" s="23"/>
-      <c r="B17" s="117"/>
+      <c r="B17" s="102"/>
       <c r="C17" s="23"/>
       <c r="D17" s="42"/>
       <c r="E17" s="51"/>
@@ -1895,52 +1895,52 @@
     </row>
     <row r="19" spans="1:54" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A19" s="23"/>
-      <c r="B19" s="113" t="s">
+      <c r="B19" s="108" t="s">
         <v>53</v>
       </c>
-      <c r="C19" s="113"/>
-      <c r="D19" s="113"/>
-      <c r="E19" s="113"/>
-      <c r="F19" s="113"/>
-      <c r="G19" s="113"/>
-      <c r="H19" s="113"/>
-      <c r="I19" s="113"/>
-      <c r="J19" s="113"/>
-      <c r="K19" s="113"/>
-      <c r="L19" s="113"/>
-      <c r="M19" s="113"/>
-      <c r="N19" s="113"/>
-      <c r="O19" s="113"/>
-      <c r="P19" s="113"/>
-      <c r="Q19" s="113"/>
-      <c r="R19" s="113"/>
-      <c r="S19" s="113"/>
-      <c r="T19" s="113"/>
-      <c r="U19" s="113"/>
-      <c r="V19" s="113"/>
-      <c r="W19" s="113"/>
-      <c r="X19" s="113"/>
-      <c r="Y19" s="113"/>
-      <c r="Z19" s="113"/>
-      <c r="AA19" s="113"/>
-      <c r="AB19" s="113"/>
-      <c r="AC19" s="113"/>
-      <c r="AD19" s="113"/>
-      <c r="AE19" s="113"/>
-      <c r="AF19" s="113"/>
-      <c r="AG19" s="113"/>
-      <c r="AH19" s="113"/>
-      <c r="AI19" s="113"/>
-      <c r="AJ19" s="113"/>
-      <c r="AK19" s="113"/>
-      <c r="AL19" s="113"/>
-      <c r="AM19" s="113"/>
-      <c r="AN19" s="113"/>
-      <c r="AO19" s="113"/>
-      <c r="AP19" s="113"/>
-      <c r="AQ19" s="113"/>
-      <c r="AR19" s="113"/>
-      <c r="AS19" s="113"/>
+      <c r="C19" s="108"/>
+      <c r="D19" s="108"/>
+      <c r="E19" s="108"/>
+      <c r="F19" s="108"/>
+      <c r="G19" s="108"/>
+      <c r="H19" s="108"/>
+      <c r="I19" s="108"/>
+      <c r="J19" s="108"/>
+      <c r="K19" s="108"/>
+      <c r="L19" s="108"/>
+      <c r="M19" s="108"/>
+      <c r="N19" s="108"/>
+      <c r="O19" s="108"/>
+      <c r="P19" s="108"/>
+      <c r="Q19" s="108"/>
+      <c r="R19" s="108"/>
+      <c r="S19" s="108"/>
+      <c r="T19" s="108"/>
+      <c r="U19" s="108"/>
+      <c r="V19" s="108"/>
+      <c r="W19" s="108"/>
+      <c r="X19" s="108"/>
+      <c r="Y19" s="108"/>
+      <c r="Z19" s="108"/>
+      <c r="AA19" s="108"/>
+      <c r="AB19" s="108"/>
+      <c r="AC19" s="108"/>
+      <c r="AD19" s="108"/>
+      <c r="AE19" s="108"/>
+      <c r="AF19" s="108"/>
+      <c r="AG19" s="108"/>
+      <c r="AH19" s="108"/>
+      <c r="AI19" s="108"/>
+      <c r="AJ19" s="108"/>
+      <c r="AK19" s="108"/>
+      <c r="AL19" s="108"/>
+      <c r="AM19" s="108"/>
+      <c r="AN19" s="108"/>
+      <c r="AO19" s="108"/>
+      <c r="AP19" s="108"/>
+      <c r="AQ19" s="108"/>
+      <c r="AR19" s="108"/>
+      <c r="AS19" s="108"/>
     </row>
     <row r="20" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A20" s="23"/>
@@ -1958,117 +1958,117 @@
       <c r="A21" s="23"/>
       <c r="B21" s="58"/>
       <c r="C21" s="11"/>
-      <c r="D21" s="114" t="s">
+      <c r="D21" s="109" t="s">
         <v>24</v>
       </c>
-      <c r="E21" s="114"/>
-      <c r="F21" s="114"/>
-      <c r="G21" s="114"/>
+      <c r="E21" s="109"/>
+      <c r="F21" s="109"/>
+      <c r="G21" s="109"/>
       <c r="H21" s="62"/>
-      <c r="I21" s="116" t="s">
+      <c r="I21" s="111" t="s">
         <v>54</v>
       </c>
-      <c r="J21" s="116"/>
-      <c r="K21" s="116"/>
-      <c r="L21" s="116"/>
-      <c r="M21" s="116"/>
-      <c r="N21" s="116"/>
-      <c r="O21" s="116"/>
-      <c r="P21" s="116"/>
-      <c r="Q21" s="116"/>
-      <c r="R21" s="116"/>
-      <c r="S21" s="116"/>
-      <c r="T21" s="116"/>
-      <c r="U21" s="116"/>
-      <c r="V21" s="116"/>
-      <c r="W21" s="116"/>
-      <c r="X21" s="116"/>
-      <c r="Y21" s="116"/>
-      <c r="Z21" s="116"/>
-      <c r="AA21" s="116"/>
-      <c r="AB21" s="116"/>
-      <c r="AC21" s="116"/>
-      <c r="AD21" s="116"/>
-      <c r="AE21" s="116"/>
-      <c r="AF21" s="116"/>
-      <c r="AG21" s="116"/>
-      <c r="AH21" s="116"/>
-      <c r="AI21" s="116"/>
-      <c r="AJ21" s="116"/>
+      <c r="J21" s="111"/>
+      <c r="K21" s="111"/>
+      <c r="L21" s="111"/>
+      <c r="M21" s="111"/>
+      <c r="N21" s="111"/>
+      <c r="O21" s="111"/>
+      <c r="P21" s="111"/>
+      <c r="Q21" s="111"/>
+      <c r="R21" s="111"/>
+      <c r="S21" s="111"/>
+      <c r="T21" s="111"/>
+      <c r="U21" s="111"/>
+      <c r="V21" s="111"/>
+      <c r="W21" s="111"/>
+      <c r="X21" s="111"/>
+      <c r="Y21" s="111"/>
+      <c r="Z21" s="111"/>
+      <c r="AA21" s="111"/>
+      <c r="AB21" s="111"/>
+      <c r="AC21" s="111"/>
+      <c r="AD21" s="111"/>
+      <c r="AE21" s="111"/>
+      <c r="AF21" s="111"/>
+      <c r="AG21" s="111"/>
+      <c r="AH21" s="111"/>
+      <c r="AI21" s="111"/>
+      <c r="AJ21" s="111"/>
       <c r="AK21" s="63"/>
-      <c r="AL21" s="115" t="s">
+      <c r="AL21" s="110" t="s">
         <v>25</v>
       </c>
-      <c r="AM21" s="115"/>
-      <c r="AN21" s="115"/>
-      <c r="AO21" s="115"/>
-      <c r="AP21" s="115"/>
-      <c r="AQ21" s="115"/>
-      <c r="AR21" s="115"/>
-      <c r="AS21" s="115"/>
-      <c r="AU21" s="100" t="s">
+      <c r="AM21" s="110"/>
+      <c r="AN21" s="110"/>
+      <c r="AO21" s="110"/>
+      <c r="AP21" s="110"/>
+      <c r="AQ21" s="110"/>
+      <c r="AR21" s="110"/>
+      <c r="AS21" s="110"/>
+      <c r="AU21" s="117" t="s">
         <v>94</v>
       </c>
-      <c r="AV21" s="101"/>
-      <c r="AW21" s="101"/>
-      <c r="AX21" s="101"/>
-      <c r="AY21" s="101"/>
-      <c r="AZ21" s="101"/>
-      <c r="BA21" s="101"/>
-      <c r="BB21" s="102"/>
+      <c r="AV21" s="118"/>
+      <c r="AW21" s="118"/>
+      <c r="AX21" s="118"/>
+      <c r="AY21" s="118"/>
+      <c r="AZ21" s="118"/>
+      <c r="BA21" s="118"/>
+      <c r="BB21" s="119"/>
     </row>
     <row r="22" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A22" s="23"/>
       <c r="B22" s="58"/>
       <c r="C22" s="11"/>
-      <c r="D22" s="122" t="s">
+      <c r="D22" s="106" t="s">
         <v>55</v>
       </c>
-      <c r="E22" s="122"/>
-      <c r="F22" s="122"/>
-      <c r="G22" s="122"/>
+      <c r="E22" s="106"/>
+      <c r="F22" s="106"/>
+      <c r="G22" s="106"/>
       <c r="H22" s="62"/>
-      <c r="I22" s="112" t="s">
+      <c r="I22" s="116" t="s">
         <v>28</v>
       </c>
-      <c r="J22" s="112"/>
-      <c r="K22" s="112"/>
-      <c r="L22" s="112"/>
-      <c r="M22" s="112"/>
-      <c r="N22" s="112"/>
-      <c r="O22" s="112"/>
-      <c r="P22" s="112"/>
-      <c r="Q22" s="112"/>
-      <c r="R22" s="112"/>
-      <c r="S22" s="112"/>
-      <c r="T22" s="112"/>
-      <c r="U22" s="112"/>
-      <c r="V22" s="112"/>
-      <c r="W22" s="112"/>
-      <c r="X22" s="112"/>
-      <c r="Y22" s="112"/>
-      <c r="Z22" s="112"/>
-      <c r="AA22" s="112"/>
-      <c r="AB22" s="112"/>
-      <c r="AC22" s="112"/>
-      <c r="AD22" s="112"/>
-      <c r="AE22" s="112"/>
-      <c r="AF22" s="112"/>
-      <c r="AG22" s="112"/>
-      <c r="AH22" s="112"/>
-      <c r="AI22" s="112"/>
-      <c r="AJ22" s="112"/>
+      <c r="J22" s="116"/>
+      <c r="K22" s="116"/>
+      <c r="L22" s="116"/>
+      <c r="M22" s="116"/>
+      <c r="N22" s="116"/>
+      <c r="O22" s="116"/>
+      <c r="P22" s="116"/>
+      <c r="Q22" s="116"/>
+      <c r="R22" s="116"/>
+      <c r="S22" s="116"/>
+      <c r="T22" s="116"/>
+      <c r="U22" s="116"/>
+      <c r="V22" s="116"/>
+      <c r="W22" s="116"/>
+      <c r="X22" s="116"/>
+      <c r="Y22" s="116"/>
+      <c r="Z22" s="116"/>
+      <c r="AA22" s="116"/>
+      <c r="AB22" s="116"/>
+      <c r="AC22" s="116"/>
+      <c r="AD22" s="116"/>
+      <c r="AE22" s="116"/>
+      <c r="AF22" s="116"/>
+      <c r="AG22" s="116"/>
+      <c r="AH22" s="116"/>
+      <c r="AI22" s="116"/>
+      <c r="AJ22" s="116"/>
       <c r="AK22" s="63"/>
-      <c r="AL22" s="108" t="s">
+      <c r="AL22" s="115" t="s">
         <v>27</v>
       </c>
-      <c r="AM22" s="108"/>
-      <c r="AN22" s="108"/>
-      <c r="AO22" s="108"/>
-      <c r="AP22" s="108"/>
-      <c r="AQ22" s="108"/>
-      <c r="AR22" s="108"/>
-      <c r="AS22" s="108"/>
+      <c r="AM22" s="115"/>
+      <c r="AN22" s="115"/>
+      <c r="AO22" s="115"/>
+      <c r="AP22" s="115"/>
+      <c r="AQ22" s="115"/>
+      <c r="AR22" s="115"/>
+      <c r="AS22" s="115"/>
       <c r="AU22" s="86">
         <v>0</v>
       </c>
@@ -2143,7 +2143,7 @@
     </row>
     <row r="24" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A24" s="23"/>
-      <c r="B24" s="117" t="s">
+      <c r="B24" s="102" t="s">
         <v>6</v>
       </c>
       <c r="C24" s="43"/>
@@ -2206,12 +2206,12 @@
     </row>
     <row r="25" spans="1:54" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A25" s="23"/>
-      <c r="B25" s="117"/>
+      <c r="B25" s="102"/>
       <c r="C25" s="23"/>
-      <c r="D25" s="107" t="s">
+      <c r="D25" s="104" t="s">
         <v>58</v>
       </c>
-      <c r="E25" s="107"/>
+      <c r="E25" s="104"/>
       <c r="F25" s="94" t="s">
         <v>56</v>
       </c>
@@ -2219,18 +2219,18 @@
         <v>1</v>
       </c>
       <c r="H25" s="68"/>
-      <c r="I25" s="109" t="s">
+      <c r="I25" s="105" t="s">
         <v>40</v>
       </c>
-      <c r="J25" s="109"/>
-      <c r="K25" s="109"/>
-      <c r="L25" s="109"/>
-      <c r="M25" s="109" t="s">
+      <c r="J25" s="105"/>
+      <c r="K25" s="105"/>
+      <c r="L25" s="105"/>
+      <c r="M25" s="105" t="s">
         <v>14</v>
       </c>
-      <c r="N25" s="109"/>
-      <c r="O25" s="109"/>
-      <c r="P25" s="109"/>
+      <c r="N25" s="105"/>
+      <c r="O25" s="105"/>
+      <c r="P25" s="105"/>
       <c r="Q25" s="94" t="s">
         <v>3</v>
       </c>
@@ -2254,16 +2254,16 @@
       <c r="AI25" s="63"/>
       <c r="AJ25" s="63"/>
       <c r="AK25" s="63"/>
-      <c r="AL25" s="109" t="s">
+      <c r="AL25" s="105" t="s">
         <v>2</v>
       </c>
-      <c r="AM25" s="109"/>
-      <c r="AN25" s="109"/>
-      <c r="AO25" s="109"/>
-      <c r="AP25" s="109"/>
-      <c r="AQ25" s="109"/>
-      <c r="AR25" s="109"/>
-      <c r="AS25" s="109"/>
+      <c r="AM25" s="105"/>
+      <c r="AN25" s="105"/>
+      <c r="AO25" s="105"/>
+      <c r="AP25" s="105"/>
+      <c r="AQ25" s="105"/>
+      <c r="AR25" s="105"/>
+      <c r="AS25" s="105"/>
       <c r="AU25" s="95" t="s">
         <v>89</v>
       </c>
@@ -2282,7 +2282,7 @@
     </row>
     <row r="26" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A26" s="23"/>
-      <c r="B26" s="117"/>
+      <c r="B26" s="102"/>
       <c r="C26" s="23"/>
       <c r="D26" s="69"/>
       <c r="E26" s="69"/>
@@ -2381,7 +2381,7 @@
     </row>
     <row r="28" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A28" s="24"/>
-      <c r="B28" s="117" t="s">
+      <c r="B28" s="102" t="s">
         <v>8</v>
       </c>
       <c r="C28" s="44"/>
@@ -2444,12 +2444,12 @@
     </row>
     <row r="29" spans="1:54" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A29" s="24"/>
-      <c r="B29" s="117"/>
+      <c r="B29" s="102"/>
       <c r="C29" s="24"/>
-      <c r="D29" s="107" t="s">
+      <c r="D29" s="104" t="s">
         <v>58</v>
       </c>
-      <c r="E29" s="107"/>
+      <c r="E29" s="104"/>
       <c r="F29" s="94" t="s">
         <v>56</v>
       </c>
@@ -2457,12 +2457,12 @@
         <v>1</v>
       </c>
       <c r="H29" s="63"/>
-      <c r="I29" s="109" t="s">
+      <c r="I29" s="105" t="s">
         <v>40</v>
       </c>
-      <c r="J29" s="109"/>
-      <c r="K29" s="109"/>
-      <c r="L29" s="109"/>
+      <c r="J29" s="105"/>
+      <c r="K29" s="105"/>
+      <c r="L29" s="105"/>
       <c r="M29" s="94" t="s">
         <v>3</v>
       </c>
@@ -2498,16 +2498,16 @@
       <c r="AI29" s="63"/>
       <c r="AJ29" s="63"/>
       <c r="AK29" s="63"/>
-      <c r="AL29" s="107" t="s">
+      <c r="AL29" s="104" t="s">
         <v>2</v>
       </c>
-      <c r="AM29" s="107"/>
-      <c r="AN29" s="107"/>
-      <c r="AO29" s="107"/>
-      <c r="AP29" s="107"/>
-      <c r="AQ29" s="107"/>
-      <c r="AR29" s="107"/>
-      <c r="AS29" s="107"/>
+      <c r="AM29" s="104"/>
+      <c r="AN29" s="104"/>
+      <c r="AO29" s="104"/>
+      <c r="AP29" s="104"/>
+      <c r="AQ29" s="104"/>
+      <c r="AR29" s="104"/>
+      <c r="AS29" s="104"/>
       <c r="AU29" s="95" t="s">
         <v>88</v>
       </c>
@@ -2517,7 +2517,7 @@
     </row>
     <row r="30" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A30" s="24"/>
-      <c r="B30" s="117"/>
+      <c r="B30" s="102"/>
       <c r="C30" s="24"/>
       <c r="D30" s="69"/>
       <c r="E30" s="69"/>
@@ -2585,7 +2585,7 @@
     </row>
     <row r="32" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A32" s="24"/>
-      <c r="B32" s="117" t="s">
+      <c r="B32" s="102" t="s">
         <v>101</v>
       </c>
       <c r="C32" s="1"/>
@@ -2640,63 +2640,63 @@
     </row>
     <row r="33" spans="1:54" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A33" s="24"/>
-      <c r="B33" s="117"/>
-      <c r="D33" s="107" t="s">
+      <c r="B33" s="102"/>
+      <c r="D33" s="104" t="s">
         <v>58</v>
       </c>
-      <c r="E33" s="107"/>
+      <c r="E33" s="104"/>
       <c r="F33" s="94" t="s">
         <v>56</v>
       </c>
       <c r="G33" s="94" t="s">
         <v>1</v>
       </c>
-      <c r="I33" s="111" t="s">
+      <c r="I33" s="103" t="s">
         <v>40</v>
       </c>
-      <c r="J33" s="111"/>
-      <c r="K33" s="111"/>
-      <c r="L33" s="111"/>
-      <c r="M33" s="111" t="s">
+      <c r="J33" s="103"/>
+      <c r="K33" s="103"/>
+      <c r="L33" s="103"/>
+      <c r="M33" s="103" t="s">
         <v>102</v>
       </c>
-      <c r="N33" s="111"/>
-      <c r="O33" s="111"/>
-      <c r="P33" s="111"/>
-      <c r="Q33" s="111" t="s">
+      <c r="N33" s="103"/>
+      <c r="O33" s="103"/>
+      <c r="P33" s="103"/>
+      <c r="Q33" s="103" t="s">
         <v>103</v>
       </c>
-      <c r="R33" s="111"/>
-      <c r="S33" s="111"/>
-      <c r="T33" s="111"/>
-      <c r="U33" s="111" t="s">
+      <c r="R33" s="103"/>
+      <c r="S33" s="103"/>
+      <c r="T33" s="103"/>
+      <c r="U33" s="103" t="s">
         <v>104</v>
       </c>
-      <c r="V33" s="111"/>
-      <c r="W33" s="111"/>
-      <c r="X33" s="111"/>
-      <c r="Y33" s="111" t="s">
+      <c r="V33" s="103"/>
+      <c r="W33" s="103"/>
+      <c r="X33" s="103"/>
+      <c r="Y33" s="103" t="s">
         <v>105</v>
       </c>
-      <c r="Z33" s="111"/>
-      <c r="AA33" s="111"/>
-      <c r="AB33" s="111"/>
-      <c r="AC33" s="111" t="s">
+      <c r="Z33" s="103"/>
+      <c r="AA33" s="103"/>
+      <c r="AB33" s="103"/>
+      <c r="AC33" s="103" t="s">
         <v>106</v>
       </c>
-      <c r="AD33" s="111"/>
-      <c r="AE33" s="111"/>
-      <c r="AF33" s="111"/>
-      <c r="AG33" s="111" t="s">
+      <c r="AD33" s="103"/>
+      <c r="AE33" s="103"/>
+      <c r="AF33" s="103"/>
+      <c r="AG33" s="103" t="s">
         <v>107</v>
       </c>
-      <c r="AH33" s="111"/>
-      <c r="AI33" s="111"/>
-      <c r="AJ33" s="111"/>
+      <c r="AH33" s="103"/>
+      <c r="AI33" s="103"/>
+      <c r="AJ33" s="103"/>
     </row>
     <row r="34" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A34" s="24"/>
-      <c r="B34" s="117"/>
+      <c r="B34" s="102"/>
       <c r="D34" s="69"/>
       <c r="E34" s="69"/>
       <c r="F34" s="70"/>
@@ -2737,7 +2737,7 @@
     </row>
     <row r="36" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A36" s="23"/>
-      <c r="B36" s="117" t="s">
+      <c r="B36" s="102" t="s">
         <v>109</v>
       </c>
       <c r="C36" s="43"/>
@@ -2800,12 +2800,12 @@
     </row>
     <row r="37" spans="1:54" ht="48.75" x14ac:dyDescent="0.25">
       <c r="A37" s="23"/>
-      <c r="B37" s="117"/>
+      <c r="B37" s="102"/>
       <c r="C37" s="23"/>
-      <c r="D37" s="107" t="s">
+      <c r="D37" s="104" t="s">
         <v>58</v>
       </c>
-      <c r="E37" s="107"/>
+      <c r="E37" s="104"/>
       <c r="F37" s="94" t="s">
         <v>56</v>
       </c>
@@ -2813,22 +2813,22 @@
         <v>1</v>
       </c>
       <c r="H37" s="96"/>
-      <c r="I37" s="109" t="s">
+      <c r="I37" s="105" t="s">
         <v>40</v>
       </c>
-      <c r="J37" s="109"/>
-      <c r="K37" s="109"/>
-      <c r="L37" s="109"/>
+      <c r="J37" s="105"/>
+      <c r="K37" s="105"/>
+      <c r="L37" s="105"/>
       <c r="M37" s="99" t="s">
         <v>14</v>
       </c>
-      <c r="N37" s="133" t="s">
+      <c r="N37" s="100" t="s">
         <v>116</v>
       </c>
-      <c r="O37" s="133" t="s">
+      <c r="O37" s="100" t="s">
         <v>116</v>
       </c>
-      <c r="P37" s="133" t="s">
+      <c r="P37" s="100" t="s">
         <v>116</v>
       </c>
       <c r="Q37" s="94" t="s">
@@ -2854,16 +2854,16 @@
       <c r="AI37" s="63"/>
       <c r="AJ37" s="63"/>
       <c r="AK37" s="63"/>
-      <c r="AL37" s="109" t="s">
+      <c r="AL37" s="105" t="s">
         <v>2</v>
       </c>
-      <c r="AM37" s="109"/>
-      <c r="AN37" s="109"/>
-      <c r="AO37" s="109"/>
-      <c r="AP37" s="109"/>
-      <c r="AQ37" s="109"/>
-      <c r="AR37" s="109"/>
-      <c r="AS37" s="109"/>
+      <c r="AM37" s="105"/>
+      <c r="AN37" s="105"/>
+      <c r="AO37" s="105"/>
+      <c r="AP37" s="105"/>
+      <c r="AQ37" s="105"/>
+      <c r="AR37" s="105"/>
+      <c r="AS37" s="105"/>
       <c r="AU37" s="95" t="s">
         <v>88</v>
       </c>
@@ -2879,7 +2879,7 @@
     </row>
     <row r="38" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A38" s="23"/>
-      <c r="B38" s="117"/>
+      <c r="B38" s="102"/>
       <c r="C38" s="23"/>
       <c r="D38" s="69"/>
       <c r="E38" s="69"/>
@@ -2977,7 +2977,7 @@
     </row>
     <row r="40" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A40" s="23"/>
-      <c r="B40" s="117" t="s">
+      <c r="B40" s="102" t="s">
         <v>43</v>
       </c>
       <c r="C40" s="1"/>
@@ -3032,38 +3032,38 @@
     </row>
     <row r="41" spans="1:54" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A41" s="5"/>
-      <c r="B41" s="117"/>
-      <c r="D41" s="107" t="s">
+      <c r="B41" s="102"/>
+      <c r="D41" s="104" t="s">
         <v>58</v>
       </c>
-      <c r="E41" s="107"/>
+      <c r="E41" s="104"/>
       <c r="F41" s="94" t="s">
         <v>56</v>
       </c>
       <c r="G41" s="94" t="s">
         <v>1</v>
       </c>
-      <c r="I41" s="111" t="s">
+      <c r="I41" s="103" t="s">
         <v>40</v>
       </c>
-      <c r="J41" s="111"/>
-      <c r="K41" s="111"/>
-      <c r="L41" s="111"/>
+      <c r="J41" s="103"/>
+      <c r="K41" s="103"/>
+      <c r="L41" s="103"/>
       <c r="M41" s="55"/>
-      <c r="AL41" s="110" t="s">
+      <c r="AL41" s="101" t="s">
         <v>2</v>
       </c>
-      <c r="AM41" s="110"/>
-      <c r="AN41" s="110"/>
-      <c r="AO41" s="110"/>
-      <c r="AP41" s="110"/>
-      <c r="AQ41" s="110"/>
-      <c r="AR41" s="110"/>
-      <c r="AS41" s="110"/>
+      <c r="AM41" s="101"/>
+      <c r="AN41" s="101"/>
+      <c r="AO41" s="101"/>
+      <c r="AP41" s="101"/>
+      <c r="AQ41" s="101"/>
+      <c r="AR41" s="101"/>
+      <c r="AS41" s="101"/>
     </row>
     <row r="42" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A42" s="5"/>
-      <c r="B42" s="117"/>
+      <c r="B42" s="102"/>
       <c r="D42" s="69"/>
       <c r="E42" s="69"/>
       <c r="F42" s="70"/>
@@ -3089,6 +3089,39 @@
     <row r="56" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="48">
+    <mergeCell ref="AU21:BB21"/>
+    <mergeCell ref="AU1:BB1"/>
+    <mergeCell ref="AV3:BB3"/>
+    <mergeCell ref="AV4:BB4"/>
+    <mergeCell ref="AV5:BB5"/>
+    <mergeCell ref="AV6:BB6"/>
+    <mergeCell ref="AV7:BB7"/>
+    <mergeCell ref="AV8:BB8"/>
+    <mergeCell ref="AV9:BB9"/>
+    <mergeCell ref="AV10:BB10"/>
+    <mergeCell ref="AL29:AS29"/>
+    <mergeCell ref="AL22:AS22"/>
+    <mergeCell ref="M25:P25"/>
+    <mergeCell ref="I25:L25"/>
+    <mergeCell ref="AL25:AS25"/>
+    <mergeCell ref="I22:AJ22"/>
+    <mergeCell ref="I29:L29"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B19:AS19"/>
+    <mergeCell ref="D21:G21"/>
+    <mergeCell ref="AL21:AS21"/>
+    <mergeCell ref="I21:AJ21"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D22:G22"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="B24:B26"/>
     <mergeCell ref="AL41:AS41"/>
     <mergeCell ref="B40:B42"/>
     <mergeCell ref="M33:P33"/>
@@ -3101,42 +3134,9 @@
     <mergeCell ref="D37:E37"/>
     <mergeCell ref="I37:L37"/>
     <mergeCell ref="AL37:AS37"/>
-    <mergeCell ref="D22:G22"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="B32:B34"/>
-    <mergeCell ref="D33:E33"/>
     <mergeCell ref="D41:E41"/>
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B19:AS19"/>
-    <mergeCell ref="D21:G21"/>
-    <mergeCell ref="AL21:AS21"/>
-    <mergeCell ref="I21:AJ21"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="AL29:AS29"/>
-    <mergeCell ref="AL22:AS22"/>
-    <mergeCell ref="M25:P25"/>
-    <mergeCell ref="I25:L25"/>
-    <mergeCell ref="AL25:AS25"/>
-    <mergeCell ref="I22:AJ22"/>
-    <mergeCell ref="I29:L29"/>
     <mergeCell ref="I33:L33"/>
     <mergeCell ref="I41:L41"/>
-    <mergeCell ref="AU21:BB21"/>
-    <mergeCell ref="AU1:BB1"/>
-    <mergeCell ref="AV3:BB3"/>
-    <mergeCell ref="AV4:BB4"/>
-    <mergeCell ref="AV5:BB5"/>
-    <mergeCell ref="AV6:BB6"/>
-    <mergeCell ref="AV7:BB7"/>
-    <mergeCell ref="AV8:BB8"/>
-    <mergeCell ref="AV9:BB9"/>
-    <mergeCell ref="AV10:BB10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3147,7 +3147,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AQ49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="W29" sqref="W29"/>
     </sheetView>
   </sheetViews>
@@ -3174,131 +3174,131 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="123"/>
-      <c r="B1" s="123"/>
-      <c r="C1" s="123"/>
-      <c r="D1" s="123"/>
-      <c r="E1" s="123"/>
-      <c r="F1" s="123"/>
-      <c r="G1" s="123"/>
-      <c r="H1" s="123"/>
-      <c r="I1" s="123"/>
-      <c r="J1" s="123"/>
-      <c r="K1" s="123"/>
-      <c r="L1" s="123"/>
-      <c r="M1" s="123"/>
-      <c r="N1" s="123"/>
-      <c r="O1" s="123"/>
-      <c r="P1" s="123"/>
-      <c r="Q1" s="123"/>
-      <c r="R1" s="123"/>
-      <c r="S1" s="123"/>
-      <c r="T1" s="123"/>
-      <c r="U1" s="123"/>
-      <c r="V1" s="123"/>
-      <c r="W1" s="123"/>
-      <c r="X1" s="123"/>
-      <c r="Y1" s="123"/>
-      <c r="Z1" s="123"/>
-      <c r="AA1" s="123"/>
-      <c r="AB1" s="123"/>
-      <c r="AC1" s="123"/>
-      <c r="AD1" s="123"/>
-      <c r="AE1" s="123"/>
-      <c r="AF1" s="123"/>
-      <c r="AG1" s="123"/>
-      <c r="AH1" s="123"/>
+      <c r="A1" s="125"/>
+      <c r="B1" s="125"/>
+      <c r="C1" s="125"/>
+      <c r="D1" s="125"/>
+      <c r="E1" s="125"/>
+      <c r="F1" s="125"/>
+      <c r="G1" s="125"/>
+      <c r="H1" s="125"/>
+      <c r="I1" s="125"/>
+      <c r="J1" s="125"/>
+      <c r="K1" s="125"/>
+      <c r="L1" s="125"/>
+      <c r="M1" s="125"/>
+      <c r="N1" s="125"/>
+      <c r="O1" s="125"/>
+      <c r="P1" s="125"/>
+      <c r="Q1" s="125"/>
+      <c r="R1" s="125"/>
+      <c r="S1" s="125"/>
+      <c r="T1" s="125"/>
+      <c r="U1" s="125"/>
+      <c r="V1" s="125"/>
+      <c r="W1" s="125"/>
+      <c r="X1" s="125"/>
+      <c r="Y1" s="125"/>
+      <c r="Z1" s="125"/>
+      <c r="AA1" s="125"/>
+      <c r="AB1" s="125"/>
+      <c r="AC1" s="125"/>
+      <c r="AD1" s="125"/>
+      <c r="AE1" s="125"/>
+      <c r="AF1" s="125"/>
+      <c r="AG1" s="125"/>
+      <c r="AH1" s="125"/>
     </row>
     <row r="2" spans="1:43" ht="21" x14ac:dyDescent="0.35">
       <c r="G2" s="7"/>
     </row>
     <row r="3" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="D3" s="118" t="s">
+      <c r="D3" s="112" t="s">
         <v>60</v>
       </c>
-      <c r="E3" s="118"/>
+      <c r="E3" s="112"/>
       <c r="F3" s="29"/>
-      <c r="G3" s="124" t="s">
+      <c r="G3" s="126" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="124"/>
-      <c r="I3" s="124"/>
-      <c r="J3" s="124"/>
-      <c r="K3" s="124"/>
-      <c r="L3" s="124"/>
-      <c r="M3" s="124"/>
-      <c r="N3" s="124"/>
-      <c r="O3" s="124"/>
-      <c r="P3" s="124"/>
-      <c r="Q3" s="124"/>
-      <c r="R3" s="124"/>
-      <c r="S3" s="124"/>
-      <c r="T3" s="124"/>
-      <c r="U3" s="124"/>
-      <c r="V3" s="124"/>
-      <c r="W3" s="124"/>
-      <c r="X3" s="124"/>
-      <c r="Y3" s="124"/>
+      <c r="H3" s="126"/>
+      <c r="I3" s="126"/>
+      <c r="J3" s="126"/>
+      <c r="K3" s="126"/>
+      <c r="L3" s="126"/>
+      <c r="M3" s="126"/>
+      <c r="N3" s="126"/>
+      <c r="O3" s="126"/>
+      <c r="P3" s="126"/>
+      <c r="Q3" s="126"/>
+      <c r="R3" s="126"/>
+      <c r="S3" s="126"/>
+      <c r="T3" s="126"/>
+      <c r="U3" s="126"/>
+      <c r="V3" s="126"/>
+      <c r="W3" s="126"/>
+      <c r="X3" s="126"/>
+      <c r="Y3" s="126"/>
       <c r="Z3" s="2"/>
-      <c r="AA3" s="125" t="s">
+      <c r="AA3" s="127" t="s">
         <v>25</v>
       </c>
-      <c r="AB3" s="125"/>
-      <c r="AC3" s="125"/>
-      <c r="AD3" s="125"/>
-      <c r="AE3" s="125"/>
-      <c r="AF3" s="125"/>
-      <c r="AG3" s="125"/>
-      <c r="AH3" s="125"/>
-      <c r="AJ3" s="100" t="s">
+      <c r="AB3" s="127"/>
+      <c r="AC3" s="127"/>
+      <c r="AD3" s="127"/>
+      <c r="AE3" s="127"/>
+      <c r="AF3" s="127"/>
+      <c r="AG3" s="127"/>
+      <c r="AH3" s="127"/>
+      <c r="AJ3" s="117" t="s">
         <v>94</v>
       </c>
-      <c r="AK3" s="101"/>
-      <c r="AL3" s="101"/>
-      <c r="AM3" s="101"/>
-      <c r="AN3" s="101"/>
-      <c r="AO3" s="101"/>
-      <c r="AP3" s="101"/>
-      <c r="AQ3" s="102"/>
+      <c r="AK3" s="118"/>
+      <c r="AL3" s="118"/>
+      <c r="AM3" s="118"/>
+      <c r="AN3" s="118"/>
+      <c r="AO3" s="118"/>
+      <c r="AP3" s="118"/>
+      <c r="AQ3" s="119"/>
     </row>
     <row r="4" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="D4" s="119" t="s">
+      <c r="D4" s="113" t="s">
         <v>61</v>
       </c>
-      <c r="E4" s="119"/>
+      <c r="E4" s="113"/>
       <c r="F4" s="29"/>
-      <c r="G4" s="126" t="s">
+      <c r="G4" s="128" t="s">
         <v>28</v>
       </c>
-      <c r="H4" s="126"/>
-      <c r="I4" s="126"/>
-      <c r="J4" s="126"/>
-      <c r="K4" s="126"/>
-      <c r="L4" s="126"/>
-      <c r="M4" s="126"/>
-      <c r="N4" s="126"/>
-      <c r="O4" s="126"/>
-      <c r="P4" s="126"/>
-      <c r="Q4" s="126"/>
-      <c r="R4" s="126"/>
-      <c r="S4" s="126"/>
-      <c r="T4" s="126"/>
-      <c r="U4" s="126"/>
-      <c r="V4" s="126"/>
-      <c r="W4" s="126"/>
-      <c r="X4" s="126"/>
-      <c r="Y4" s="126"/>
+      <c r="H4" s="128"/>
+      <c r="I4" s="128"/>
+      <c r="J4" s="128"/>
+      <c r="K4" s="128"/>
+      <c r="L4" s="128"/>
+      <c r="M4" s="128"/>
+      <c r="N4" s="128"/>
+      <c r="O4" s="128"/>
+      <c r="P4" s="128"/>
+      <c r="Q4" s="128"/>
+      <c r="R4" s="128"/>
+      <c r="S4" s="128"/>
+      <c r="T4" s="128"/>
+      <c r="U4" s="128"/>
+      <c r="V4" s="128"/>
+      <c r="W4" s="128"/>
+      <c r="X4" s="128"/>
+      <c r="Y4" s="128"/>
       <c r="Z4" s="31"/>
-      <c r="AA4" s="127" t="s">
+      <c r="AA4" s="129" t="s">
         <v>27</v>
       </c>
-      <c r="AB4" s="127"/>
-      <c r="AC4" s="127"/>
-      <c r="AD4" s="127"/>
-      <c r="AE4" s="127"/>
-      <c r="AF4" s="127"/>
-      <c r="AG4" s="127"/>
-      <c r="AH4" s="127"/>
+      <c r="AB4" s="129"/>
+      <c r="AC4" s="129"/>
+      <c r="AD4" s="129"/>
+      <c r="AE4" s="129"/>
+      <c r="AF4" s="129"/>
+      <c r="AG4" s="129"/>
+      <c r="AH4" s="129"/>
       <c r="AJ4" s="86">
         <v>0</v>
       </c>
@@ -3414,7 +3414,7 @@
     </row>
     <row r="7" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A7" s="23"/>
-      <c r="B7" s="117" t="s">
+      <c r="B7" s="102" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="43"/>
@@ -3466,19 +3466,19 @@
     </row>
     <row r="8" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A8" s="23"/>
-      <c r="B8" s="117"/>
+      <c r="B8" s="102"/>
       <c r="C8" s="23"/>
-      <c r="D8" s="111" t="s">
+      <c r="D8" s="103" t="s">
         <v>62</v>
       </c>
-      <c r="E8" s="111"/>
+      <c r="E8" s="103"/>
       <c r="F8" s="28"/>
-      <c r="G8" s="111" t="s">
+      <c r="G8" s="103" t="s">
         <v>40</v>
       </c>
-      <c r="H8" s="111"/>
-      <c r="I8" s="111"/>
-      <c r="J8" s="111"/>
+      <c r="H8" s="103"/>
+      <c r="I8" s="103"/>
+      <c r="J8" s="103"/>
       <c r="K8" s="16" t="s">
         <v>5</v>
       </c>
@@ -3488,25 +3488,25 @@
       <c r="M8" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="N8" s="111" t="s">
+      <c r="N8" s="103" t="s">
         <v>14</v>
       </c>
-      <c r="O8" s="111"/>
-      <c r="P8" s="111"/>
-      <c r="Q8" s="111"/>
+      <c r="O8" s="103"/>
+      <c r="P8" s="103"/>
+      <c r="Q8" s="103"/>
       <c r="R8" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="AA8" s="110" t="s">
+      <c r="AA8" s="101" t="s">
         <v>2</v>
       </c>
-      <c r="AB8" s="110"/>
-      <c r="AC8" s="110"/>
-      <c r="AD8" s="110"/>
-      <c r="AE8" s="110"/>
-      <c r="AF8" s="110"/>
-      <c r="AG8" s="110"/>
-      <c r="AH8" s="110"/>
+      <c r="AB8" s="101"/>
+      <c r="AC8" s="101"/>
+      <c r="AD8" s="101"/>
+      <c r="AE8" s="101"/>
+      <c r="AF8" s="101"/>
+      <c r="AG8" s="101"/>
+      <c r="AH8" s="101"/>
       <c r="AJ8" t="s">
         <v>89</v>
       </c>
@@ -3525,7 +3525,7 @@
     </row>
     <row r="9" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A9" s="23"/>
-      <c r="B9" s="117"/>
+      <c r="B9" s="102"/>
       <c r="C9" s="23"/>
       <c r="D9" s="12"/>
       <c r="E9" s="13"/>
@@ -3583,7 +3583,7 @@
     </row>
     <row r="11" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A11" s="24"/>
-      <c r="B11" s="117" t="s">
+      <c r="B11" s="102" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="44"/>
@@ -3635,19 +3635,19 @@
     </row>
     <row r="12" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A12" s="24"/>
-      <c r="B12" s="117"/>
+      <c r="B12" s="102"/>
       <c r="C12" s="24"/>
-      <c r="D12" s="111" t="s">
+      <c r="D12" s="103" t="s">
         <v>63</v>
       </c>
-      <c r="E12" s="111"/>
+      <c r="E12" s="103"/>
       <c r="F12" s="28"/>
-      <c r="G12" s="111" t="s">
+      <c r="G12" s="103" t="s">
         <v>40</v>
       </c>
-      <c r="H12" s="111"/>
-      <c r="I12" s="111"/>
-      <c r="J12" s="111"/>
+      <c r="H12" s="103"/>
+      <c r="I12" s="103"/>
+      <c r="J12" s="103"/>
       <c r="K12" s="16" t="s">
         <v>5</v>
       </c>
@@ -3660,16 +3660,16 @@
       <c r="N12" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="AA12" s="110" t="s">
+      <c r="AA12" s="101" t="s">
         <v>2</v>
       </c>
-      <c r="AB12" s="110"/>
-      <c r="AC12" s="110"/>
-      <c r="AD12" s="110"/>
-      <c r="AE12" s="110"/>
-      <c r="AF12" s="110"/>
-      <c r="AG12" s="110"/>
-      <c r="AH12" s="110"/>
+      <c r="AB12" s="101"/>
+      <c r="AC12" s="101"/>
+      <c r="AD12" s="101"/>
+      <c r="AE12" s="101"/>
+      <c r="AF12" s="101"/>
+      <c r="AG12" s="101"/>
+      <c r="AH12" s="101"/>
       <c r="AJ12" t="s">
         <v>88</v>
       </c>
@@ -3679,7 +3679,7 @@
     </row>
     <row r="13" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A13" s="24"/>
-      <c r="B13" s="117"/>
+      <c r="B13" s="102"/>
       <c r="C13" s="24"/>
       <c r="D13" s="30"/>
       <c r="E13" s="13"/>
@@ -3722,7 +3722,7 @@
     </row>
     <row r="15" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A15" s="24"/>
-      <c r="B15" s="117" t="s">
+      <c r="B15" s="102" t="s">
         <v>7</v>
       </c>
       <c r="C15" s="44"/>
@@ -3766,32 +3766,32 @@
     </row>
     <row r="16" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A16" s="24"/>
-      <c r="B16" s="117"/>
+      <c r="B16" s="102"/>
       <c r="C16" s="24"/>
-      <c r="D16" s="111" t="s">
+      <c r="D16" s="103" t="s">
         <v>64</v>
       </c>
-      <c r="E16" s="111"/>
+      <c r="E16" s="103"/>
       <c r="F16" s="28"/>
-      <c r="G16" s="111" t="s">
+      <c r="G16" s="103" t="s">
         <v>40</v>
       </c>
-      <c r="H16" s="111"/>
-      <c r="I16" s="111"/>
-      <c r="J16" s="111"/>
-      <c r="K16" s="111" t="s">
+      <c r="H16" s="103"/>
+      <c r="I16" s="103"/>
+      <c r="J16" s="103"/>
+      <c r="K16" s="103" t="s">
         <v>14</v>
       </c>
-      <c r="L16" s="111"/>
-      <c r="M16" s="111"/>
-      <c r="N16" s="111"/>
+      <c r="L16" s="103"/>
+      <c r="M16" s="103"/>
+      <c r="N16" s="103"/>
       <c r="O16" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A17" s="24"/>
-      <c r="B17" s="117"/>
+      <c r="B17" s="102"/>
       <c r="C17" s="24"/>
       <c r="D17" s="30"/>
       <c r="E17" s="13"/>
@@ -3821,7 +3821,7 @@
     </row>
     <row r="19" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A19" s="23"/>
-      <c r="B19" s="117" t="s">
+      <c r="B19" s="102" t="s">
         <v>9</v>
       </c>
       <c r="C19" s="43"/>
@@ -3865,19 +3865,19 @@
     </row>
     <row r="20" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
-      <c r="B20" s="117"/>
+      <c r="B20" s="102"/>
       <c r="C20" s="5"/>
-      <c r="D20" s="111" t="s">
+      <c r="D20" s="103" t="s">
         <v>65</v>
       </c>
-      <c r="E20" s="111"/>
+      <c r="E20" s="103"/>
       <c r="F20" s="28"/>
-      <c r="G20" s="111" t="s">
+      <c r="G20" s="103" t="s">
         <v>40</v>
       </c>
-      <c r="H20" s="111"/>
-      <c r="I20" s="111"/>
-      <c r="J20" s="111"/>
+      <c r="H20" s="103"/>
+      <c r="I20" s="103"/>
+      <c r="J20" s="103"/>
       <c r="K20" s="16" t="s">
         <v>5</v>
       </c>
@@ -3895,23 +3895,23 @@
       </c>
       <c r="P20" s="55"/>
       <c r="Q20" s="55"/>
-      <c r="AA20" s="110" t="s">
+      <c r="AA20" s="101" t="s">
         <v>2</v>
       </c>
-      <c r="AB20" s="110"/>
-      <c r="AC20" s="110"/>
-      <c r="AD20" s="110"/>
-      <c r="AE20" s="110"/>
-      <c r="AF20" s="110"/>
-      <c r="AG20" s="110"/>
-      <c r="AH20" s="110"/>
+      <c r="AB20" s="101"/>
+      <c r="AC20" s="101"/>
+      <c r="AD20" s="101"/>
+      <c r="AE20" s="101"/>
+      <c r="AF20" s="101"/>
+      <c r="AG20" s="101"/>
+      <c r="AH20" s="101"/>
       <c r="AJ20" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
-      <c r="B21" s="117"/>
+      <c r="B21" s="102"/>
       <c r="C21" s="5"/>
       <c r="D21" s="30"/>
       <c r="E21" s="13"/>
@@ -3944,7 +3944,7 @@
     </row>
     <row r="23" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
-      <c r="B23" s="117" t="s">
+      <c r="B23" s="102" t="s">
         <v>122</v>
       </c>
       <c r="C23" s="43"/>
@@ -3988,21 +3988,21 @@
     </row>
     <row r="24" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
-      <c r="B24" s="117"/>
+      <c r="B24" s="102"/>
       <c r="C24" s="5"/>
-      <c r="D24" s="111"/>
-      <c r="E24" s="111"/>
+      <c r="D24" s="103"/>
+      <c r="E24" s="103"/>
       <c r="F24" s="28"/>
-      <c r="G24" s="111" t="s">
+      <c r="G24" s="103" t="s">
         <v>40</v>
       </c>
-      <c r="H24" s="111"/>
-      <c r="I24" s="111"/>
-      <c r="J24" s="111"/>
+      <c r="H24" s="103"/>
+      <c r="I24" s="103"/>
+      <c r="J24" s="103"/>
     </row>
     <row r="25" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
-      <c r="B25" s="117"/>
+      <c r="B25" s="102"/>
       <c r="C25" s="5"/>
       <c r="D25" s="30"/>
       <c r="E25" s="13"/>
@@ -4019,7 +4019,7 @@
     </row>
     <row r="27" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
-      <c r="B27" s="117" t="s">
+      <c r="B27" s="102" t="s">
         <v>117</v>
       </c>
       <c r="C27" s="43"/>
@@ -4063,19 +4063,19 @@
     </row>
     <row r="28" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
-      <c r="B28" s="117"/>
+      <c r="B28" s="102"/>
       <c r="C28" s="5"/>
-      <c r="D28" s="111" t="s">
+      <c r="D28" s="103" t="s">
         <v>120</v>
       </c>
-      <c r="E28" s="111"/>
+      <c r="E28" s="103"/>
       <c r="F28" s="28"/>
-      <c r="G28" s="111" t="s">
+      <c r="G28" s="103" t="s">
         <v>40</v>
       </c>
-      <c r="H28" s="111"/>
-      <c r="I28" s="111"/>
-      <c r="J28" s="111"/>
+      <c r="H28" s="103"/>
+      <c r="I28" s="103"/>
+      <c r="J28" s="103"/>
       <c r="K28" s="16" t="s">
         <v>5</v>
       </c>
@@ -4091,7 +4091,7 @@
     </row>
     <row r="29" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
-      <c r="B29" s="117"/>
+      <c r="B29" s="102"/>
       <c r="C29" s="5"/>
       <c r="D29" s="30"/>
       <c r="E29" s="13"/>
@@ -4112,7 +4112,7 @@
     </row>
     <row r="31" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
-      <c r="B31" s="117" t="s">
+      <c r="B31" s="102" t="s">
         <v>119</v>
       </c>
       <c r="C31" s="43"/>
@@ -4156,26 +4156,26 @@
     </row>
     <row r="32" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
-      <c r="B32" s="117"/>
+      <c r="B32" s="102"/>
       <c r="C32" s="5"/>
-      <c r="D32" s="111" t="s">
+      <c r="D32" s="103" t="s">
         <v>121</v>
       </c>
-      <c r="E32" s="111"/>
+      <c r="E32" s="103"/>
       <c r="F32" s="28"/>
-      <c r="G32" s="111" t="s">
+      <c r="G32" s="103" t="s">
         <v>40</v>
       </c>
-      <c r="H32" s="111"/>
-      <c r="I32" s="111"/>
-      <c r="J32" s="111"/>
+      <c r="H32" s="103"/>
+      <c r="I32" s="103"/>
+      <c r="J32" s="103"/>
       <c r="K32" s="16" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="33" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
-      <c r="B33" s="117"/>
+      <c r="B33" s="102"/>
       <c r="C33" s="5"/>
       <c r="D33" s="30"/>
       <c r="E33" s="13"/>
@@ -4192,7 +4192,7 @@
       <c r="C34" s="5"/>
     </row>
     <row r="35" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="B35" s="117" t="s">
+      <c r="B35" s="102" t="s">
         <v>10</v>
       </c>
       <c r="C35" s="1"/>
@@ -4235,22 +4235,22 @@
       <c r="AH35" s="1"/>
     </row>
     <row r="36" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="B36" s="117"/>
-      <c r="D36" s="111" t="s">
+      <c r="B36" s="102"/>
+      <c r="D36" s="103" t="s">
         <v>66</v>
       </c>
-      <c r="E36" s="111"/>
+      <c r="E36" s="103"/>
       <c r="F36" s="28"/>
-      <c r="G36" s="111" t="s">
+      <c r="G36" s="103" t="s">
         <v>40</v>
       </c>
-      <c r="H36" s="111"/>
-      <c r="I36" s="111"/>
-      <c r="J36" s="111"/>
-      <c r="K36" s="111" t="s">
+      <c r="H36" s="103"/>
+      <c r="I36" s="103"/>
+      <c r="J36" s="103"/>
+      <c r="K36" s="103" t="s">
         <v>15</v>
       </c>
-      <c r="L36" s="111"/>
+      <c r="L36" s="103"/>
       <c r="M36" s="16" t="s">
         <v>16</v>
       </c>
@@ -4260,19 +4260,19 @@
       <c r="O36" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="AA36" s="110" t="s">
+      <c r="AA36" s="101" t="s">
         <v>2</v>
       </c>
-      <c r="AB36" s="110"/>
-      <c r="AC36" s="110"/>
-      <c r="AD36" s="110"/>
-      <c r="AE36" s="110"/>
-      <c r="AF36" s="110"/>
-      <c r="AG36" s="110"/>
-      <c r="AH36" s="110"/>
+      <c r="AB36" s="101"/>
+      <c r="AC36" s="101"/>
+      <c r="AD36" s="101"/>
+      <c r="AE36" s="101"/>
+      <c r="AF36" s="101"/>
+      <c r="AG36" s="101"/>
+      <c r="AH36" s="101"/>
     </row>
     <row r="37" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="B37" s="117"/>
+      <c r="B37" s="102"/>
       <c r="D37" s="30"/>
       <c r="E37" s="13"/>
       <c r="F37" s="27"/>
@@ -4295,7 +4295,7 @@
       <c r="AH37" s="14"/>
     </row>
     <row r="39" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="B39" s="117" t="s">
+      <c r="B39" s="102" t="s">
         <v>11</v>
       </c>
       <c r="C39" s="1"/>
@@ -4338,22 +4338,22 @@
       <c r="AH39" s="1"/>
     </row>
     <row r="40" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="B40" s="117"/>
-      <c r="D40" s="111" t="s">
+      <c r="B40" s="102"/>
+      <c r="D40" s="103" t="s">
         <v>67</v>
       </c>
-      <c r="E40" s="111"/>
+      <c r="E40" s="103"/>
       <c r="F40" s="28"/>
-      <c r="G40" s="111" t="s">
+      <c r="G40" s="103" t="s">
         <v>40</v>
       </c>
-      <c r="H40" s="111"/>
-      <c r="I40" s="111"/>
-      <c r="J40" s="111"/>
-      <c r="K40" s="111" t="s">
+      <c r="H40" s="103"/>
+      <c r="I40" s="103"/>
+      <c r="J40" s="103"/>
+      <c r="K40" s="103" t="s">
         <v>15</v>
       </c>
-      <c r="L40" s="111"/>
+      <c r="L40" s="103"/>
       <c r="M40" s="16" t="s">
         <v>16</v>
       </c>
@@ -4369,19 +4369,19 @@
       <c r="Q40" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="AA40" s="110" t="s">
+      <c r="AA40" s="101" t="s">
         <v>2</v>
       </c>
-      <c r="AB40" s="110"/>
-      <c r="AC40" s="110"/>
-      <c r="AD40" s="110"/>
-      <c r="AE40" s="110"/>
-      <c r="AF40" s="110"/>
-      <c r="AG40" s="110"/>
-      <c r="AH40" s="110"/>
+      <c r="AB40" s="101"/>
+      <c r="AC40" s="101"/>
+      <c r="AD40" s="101"/>
+      <c r="AE40" s="101"/>
+      <c r="AF40" s="101"/>
+      <c r="AG40" s="101"/>
+      <c r="AH40" s="101"/>
     </row>
     <row r="41" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="B41" s="117"/>
+      <c r="B41" s="102"/>
       <c r="D41" s="30"/>
       <c r="E41" s="13"/>
       <c r="F41" s="27"/>
@@ -4406,7 +4406,7 @@
       <c r="AH41" s="14"/>
     </row>
     <row r="43" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="B43" s="117" t="s">
+      <c r="B43" s="102" t="s">
         <v>12</v>
       </c>
       <c r="C43" s="1"/>
@@ -4449,54 +4449,54 @@
       <c r="AH43" s="1"/>
     </row>
     <row r="44" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="B44" s="117"/>
-      <c r="D44" s="111" t="s">
+      <c r="B44" s="102"/>
+      <c r="D44" s="103" t="s">
         <v>68</v>
       </c>
-      <c r="E44" s="111"/>
+      <c r="E44" s="103"/>
       <c r="F44" s="28"/>
-      <c r="G44" s="111" t="s">
+      <c r="G44" s="103" t="s">
         <v>40</v>
       </c>
-      <c r="H44" s="111"/>
-      <c r="I44" s="111"/>
-      <c r="J44" s="111"/>
-      <c r="K44" s="121" t="s">
+      <c r="H44" s="103"/>
+      <c r="I44" s="103"/>
+      <c r="J44" s="103"/>
+      <c r="K44" s="124" t="s">
         <v>21</v>
       </c>
-      <c r="L44" s="121"/>
-      <c r="M44" s="121"/>
-      <c r="N44" s="121"/>
-      <c r="O44" s="121"/>
-      <c r="P44" s="121"/>
-      <c r="Q44" s="121" t="s">
+      <c r="L44" s="124"/>
+      <c r="M44" s="124"/>
+      <c r="N44" s="124"/>
+      <c r="O44" s="124"/>
+      <c r="P44" s="124"/>
+      <c r="Q44" s="124" t="s">
         <v>22</v>
       </c>
-      <c r="R44" s="121"/>
-      <c r="S44" s="121"/>
-      <c r="T44" s="121"/>
-      <c r="U44" s="121"/>
-      <c r="V44" s="121"/>
-      <c r="W44" s="111" t="s">
+      <c r="R44" s="124"/>
+      <c r="S44" s="124"/>
+      <c r="T44" s="124"/>
+      <c r="U44" s="124"/>
+      <c r="V44" s="124"/>
+      <c r="W44" s="103" t="s">
         <v>23</v>
       </c>
-      <c r="X44" s="111"/>
+      <c r="X44" s="103"/>
       <c r="Y44" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="AA44" s="110" t="s">
+      <c r="AA44" s="101" t="s">
         <v>2</v>
       </c>
-      <c r="AB44" s="110"/>
-      <c r="AC44" s="110"/>
-      <c r="AD44" s="110"/>
-      <c r="AE44" s="110"/>
-      <c r="AF44" s="110"/>
-      <c r="AG44" s="110"/>
-      <c r="AH44" s="110"/>
+      <c r="AB44" s="101"/>
+      <c r="AC44" s="101"/>
+      <c r="AD44" s="101"/>
+      <c r="AE44" s="101"/>
+      <c r="AF44" s="101"/>
+      <c r="AG44" s="101"/>
+      <c r="AH44" s="101"/>
     </row>
     <row r="45" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="B45" s="117"/>
+      <c r="B45" s="102"/>
       <c r="D45" s="30"/>
       <c r="E45" s="13"/>
       <c r="F45" s="27"/>
@@ -4529,7 +4529,7 @@
       <c r="AH45" s="14"/>
     </row>
     <row r="47" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="117" t="s">
+      <c r="B47" s="102" t="s">
         <v>43</v>
       </c>
       <c r="C47" s="1"/>
@@ -4572,29 +4572,29 @@
       <c r="AH47" s="1"/>
     </row>
     <row r="48" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="B48" s="117"/>
+      <c r="B48" s="102"/>
       <c r="D48" s="9"/>
       <c r="E48" s="9"/>
       <c r="F48" s="28"/>
-      <c r="G48" s="111" t="s">
+      <c r="G48" s="103" t="s">
         <v>40</v>
       </c>
-      <c r="H48" s="111"/>
-      <c r="I48" s="111"/>
-      <c r="J48" s="111"/>
-      <c r="AA48" s="110" t="s">
+      <c r="H48" s="103"/>
+      <c r="I48" s="103"/>
+      <c r="J48" s="103"/>
+      <c r="AA48" s="101" t="s">
         <v>2</v>
       </c>
-      <c r="AB48" s="110"/>
-      <c r="AC48" s="110"/>
-      <c r="AD48" s="110"/>
-      <c r="AE48" s="110"/>
-      <c r="AF48" s="110"/>
-      <c r="AG48" s="110"/>
-      <c r="AH48" s="110"/>
+      <c r="AB48" s="101"/>
+      <c r="AC48" s="101"/>
+      <c r="AD48" s="101"/>
+      <c r="AE48" s="101"/>
+      <c r="AF48" s="101"/>
+      <c r="AG48" s="101"/>
+      <c r="AH48" s="101"/>
     </row>
     <row r="49" spans="2:34" x14ac:dyDescent="0.25">
-      <c r="B49" s="117"/>
+      <c r="B49" s="102"/>
       <c r="D49" s="30"/>
       <c r="E49" s="13"/>
       <c r="F49" s="27"/>
@@ -4613,11 +4613,29 @@
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="G28:J28"/>
-    <mergeCell ref="B31:B33"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="G32:J32"/>
-    <mergeCell ref="AJ3:AQ3"/>
+    <mergeCell ref="A1:AH1"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="G3:Y3"/>
+    <mergeCell ref="AA3:AH3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="G4:Y4"/>
+    <mergeCell ref="AA4:AH4"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="G8:J8"/>
+    <mergeCell ref="N8:Q8"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="G36:J36"/>
+    <mergeCell ref="K36:L36"/>
+    <mergeCell ref="AA36:AH36"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="G24:J24"/>
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="D28:E28"/>
     <mergeCell ref="B47:B49"/>
     <mergeCell ref="G48:J48"/>
     <mergeCell ref="AA48:AH48"/>
@@ -4633,20 +4651,14 @@
     <mergeCell ref="Q44:V44"/>
     <mergeCell ref="W44:X44"/>
     <mergeCell ref="AA44:AH44"/>
+    <mergeCell ref="G28:J28"/>
+    <mergeCell ref="B31:B33"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="G32:J32"/>
+    <mergeCell ref="AJ3:AQ3"/>
     <mergeCell ref="B19:B21"/>
     <mergeCell ref="G20:J20"/>
     <mergeCell ref="AA20:AH20"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="G36:J36"/>
-    <mergeCell ref="K36:L36"/>
-    <mergeCell ref="AA36:AH36"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="G24:J24"/>
-    <mergeCell ref="B27:B29"/>
-    <mergeCell ref="D28:E28"/>
     <mergeCell ref="AA8:AH8"/>
     <mergeCell ref="B15:B17"/>
     <mergeCell ref="G16:J16"/>
@@ -4655,18 +4667,6 @@
     <mergeCell ref="G12:J12"/>
     <mergeCell ref="AA12:AH12"/>
     <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="G8:J8"/>
-    <mergeCell ref="N8:Q8"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="A1:AH1"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="G3:Y3"/>
-    <mergeCell ref="AA3:AH3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="G4:Y4"/>
-    <mergeCell ref="AA4:AH4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4837,7 +4837,7 @@
       <c r="E11" s="26"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="128" t="s">
+      <c r="A12" s="130" t="s">
         <v>59</v>
       </c>
       <c r="B12" s="26" t="s">
@@ -4854,7 +4854,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="129"/>
+      <c r="A13" s="131"/>
       <c r="B13" s="45" t="s">
         <v>77</v>
       </c>
@@ -4869,7 +4869,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="129"/>
+      <c r="A14" s="131"/>
       <c r="B14" s="45" t="s">
         <v>73</v>
       </c>
@@ -4880,7 +4880,7 @@
       <c r="E14" s="48"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="129"/>
+      <c r="A15" s="131"/>
       <c r="B15" s="45" t="s">
         <v>74</v>
       </c>
@@ -4891,7 +4891,7 @@
       <c r="E15" s="48"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="129"/>
+      <c r="A16" s="131"/>
       <c r="B16" s="45" t="s">
         <v>75</v>
       </c>
@@ -4906,7 +4906,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="130"/>
+      <c r="A17" s="132"/>
       <c r="B17" s="26" t="s">
         <v>76</v>
       </c>
@@ -4940,8 +4940,8 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D28" s="2"/>
-      <c r="E28" s="131"/>
-      <c r="F28" s="131"/>
+      <c r="E28" s="133"/>
+      <c r="F28" s="133"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>

</xml_diff>